<commit_message>
update figs 1-4 and equity to work with new data sets
</commit_message>
<xml_diff>
--- a/data/scenarios_assessed.xlsx
+++ b/data/scenarios_assessed.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="904" documentId="11_AB6950C68BE577815F655C903F0D020999345216" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F85C1E5B-6DE3-460E-A591-1FB9D9D735FE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="core" sheetId="9" r:id="rId1"/>
@@ -703,12 +703,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -719,6 +713,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1739,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5041401-7584-4CC5-BF57-23EAA11913DE}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,7 +1760,7 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="39" t="s">
@@ -2220,7 +2220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FADE4FE-2402-42D1-ABBB-07D12D880BB0}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2412,22 +2412,22 @@
       <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="63" t="s">
+      <c r="D8" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="61" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="20"/>
@@ -2436,22 +2436,22 @@
       <c r="A9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="63" t="s">
+      <c r="D9" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="61" t="s">
         <v>52</v>
       </c>
       <c r="H9" s="20" t="s">
@@ -2462,22 +2462,22 @@
       <c r="A10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="63" t="s">
+      <c r="D10" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="61" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="20" t="s">
@@ -2485,54 +2485,54 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="64" t="s">
+      <c r="A11" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="64" t="s">
+      <c r="D11" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="57" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="61" t="s">
+      <c r="A12" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="61" t="s">
+      <c r="D12" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="62" t="s">
+      <c r="H12" s="60" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3338,22 +3338,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="42" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="55" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="55" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="55" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="56"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" s="42" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
@@ -3467,26 +3467,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c726f2c6-9946-4811-9843-facded7c8750">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="767e6690-7a14-4d32-91ce-7a1186ad202b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB8E7E01FDBC894A8118D024CD01B609" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0070e2b1b8f6382a0efab2c59a69bc3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c726f2c6-9946-4811-9843-facded7c8750" xmlns:ns3="767e6690-7a14-4d32-91ce-7a1186ad202b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83e8106f57ea953c7fa3fea1e1e6268e" ns2:_="" ns3:_="">
     <xsd:import namespace="c726f2c6-9946-4811-9843-facded7c8750"/>
@@ -3717,26 +3697,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1876BA54-5C2B-401A-9CE0-0E1E96E100C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c726f2c6-9946-4811-9843-facded7c8750"/>
-    <ds:schemaRef ds:uri="767e6690-7a14-4d32-91ce-7a1186ad202b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35AE2B60-10BF-40CC-A4A2-790A1E73F5CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c726f2c6-9946-4811-9843-facded7c8750">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="767e6690-7a14-4d32-91ce-7a1186ad202b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F051516-B1EA-48A8-BD46-1E5A40AC7133}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3753,4 +3734,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35AE2B60-10BF-40CC-A4A2-790A1E73F5CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1876BA54-5C2B-401A-9CE0-0E1E96E100C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c726f2c6-9946-4811-9843-facded7c8750"/>
+    <ds:schemaRef ds:uri="767e6690-7a14-4d32-91ce-7a1186ad202b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>